<commit_message>
Issue creators can create Epic, excel reader starts calling issue creation subs
</commit_message>
<xml_diff>
--- a/testexcel.xlsx
+++ b/testexcel.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,9 +223,7 @@
       <c r="C3" s="1" t="n">
         <v>324</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>253</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="n">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Example excel parsing and Epic creations to target Jira Cloud project works ok
</commit_message>
<xml_diff>
--- a/testexcel.xlsx
+++ b/testexcel.xlsx
@@ -20,57 +20,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Key-id</t>
   </si>
   <si>
-    <t xml:space="preserve">toka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kolmas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neljas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viides</t>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POINTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRASUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPTION</t>
   </si>
   <si>
     <t xml:space="preserve">AB-1</t>
   </si>
   <si>
+    <t xml:space="preserve">https://qwerty.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarina jatkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tassa on tarinaa</t>
+  </si>
+  <si>
     <t xml:space="preserve">AB-2</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://yle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.fi</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">kissa naukuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blaa blaadi </t>
+  </si>
+  <si>
     <t xml:space="preserve">AB-3</t>
   </si>
   <si>
-    <t xml:space="preserve">bneljas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cneeljas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dneljas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eneljas</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://mtv3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.fi</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">koira haukkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupu hupu lupi</t>
   </si>
   <si>
     <t xml:space="preserve">AB-4</t>
   </si>
   <si>
-    <t xml:space="preserve">bbb.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ccc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dd.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ee.com</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://bbb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.com</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">pupu paukkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekstii tekstii blaa</t>
   </si>
 </sst>
 </file>
@@ -80,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,6 +170,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,12 +221,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,13 +251,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -195,74 +275,96 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>234</v>
+        <v>3.5</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>11</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>324</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="n">
-        <v>34</v>
+        <v>4.7</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>6789</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://yle"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://mtv3"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://bbb"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>